<commit_message>
Fixed disable value and added comments
</commit_message>
<xml_diff>
--- a/Final Project Gantt Chart.xlsx
+++ b/Final Project Gantt Chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD0A2E5-8C63-44CB-BD47-48EB5C2D089D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB3D28C-DA82-4730-B3C9-50D946EAE5D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="11733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="34400" windowHeight="12740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -938,6 +938,18 @@
     <xf numFmtId="164" fontId="23" fillId="10" borderId="2" xfId="10" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -945,18 +957,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1527,25 +1527,25 @@
   <dimension ref="A1:BL37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.703125" style="38" customWidth="1"/>
-    <col min="2" max="2" width="36.3515625" customWidth="1"/>
-    <col min="3" max="3" width="15.64453125" customWidth="1"/>
-    <col min="4" max="4" width="10.703125" customWidth="1"/>
-    <col min="5" max="5" width="10.46875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.46875" customWidth="1"/>
-    <col min="7" max="7" width="2.703125" customWidth="1"/>
-    <col min="8" max="8" width="6.17578125" hidden="1" customWidth="1"/>
-    <col min="9" max="64" width="2.52734375" customWidth="1"/>
-    <col min="69" max="70" width="10.29296875"/>
+    <col min="1" max="1" width="2.7265625" style="38" customWidth="1"/>
+    <col min="2" max="2" width="36.36328125" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" customWidth="1"/>
+    <col min="7" max="7" width="2.7265625" customWidth="1"/>
+    <col min="8" max="8" width="6.1796875" hidden="1" customWidth="1"/>
+    <col min="9" max="64" width="2.54296875" customWidth="1"/>
+    <col min="69" max="70" width="10.26953125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.95">
+    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A1" s="39" t="s">
         <v>28</v>
       </c>
@@ -1559,7 +1559,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="14"/>
     </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="38" t="s">
         <v>23</v>
       </c>
@@ -1568,123 +1568,123 @@
       </c>
       <c r="I2" s="41"/>
     </row>
-    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="38" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="45"/>
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="86"/>
-      <c r="E3" s="91">
+      <c r="D3" s="90"/>
+      <c r="E3" s="88">
         <f>DATE(2020, 10, 19)</f>
         <v>44123</v>
       </c>
-      <c r="F3" s="91"/>
-    </row>
-    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="F3" s="88"/>
+    </row>
+    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="85" t="s">
+      <c r="C4" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="86"/>
+      <c r="D4" s="90"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="88">
+      <c r="I4" s="85">
         <f>I5</f>
         <v>44122</v>
       </c>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="88">
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="85">
         <f>P5</f>
         <v>44129</v>
       </c>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="89"/>
-      <c r="T4" s="89"/>
-      <c r="U4" s="89"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="88">
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86"/>
+      <c r="S4" s="86"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="86"/>
+      <c r="V4" s="87"/>
+      <c r="W4" s="85">
         <f>W5</f>
         <v>44136</v>
       </c>
-      <c r="X4" s="89"/>
-      <c r="Y4" s="89"/>
-      <c r="Z4" s="89"/>
-      <c r="AA4" s="89"/>
-      <c r="AB4" s="89"/>
-      <c r="AC4" s="90"/>
-      <c r="AD4" s="88">
+      <c r="X4" s="86"/>
+      <c r="Y4" s="86"/>
+      <c r="Z4" s="86"/>
+      <c r="AA4" s="86"/>
+      <c r="AB4" s="86"/>
+      <c r="AC4" s="87"/>
+      <c r="AD4" s="85">
         <f>AD5</f>
         <v>44143</v>
       </c>
-      <c r="AE4" s="89"/>
-      <c r="AF4" s="89"/>
-      <c r="AG4" s="89"/>
-      <c r="AH4" s="89"/>
-      <c r="AI4" s="89"/>
-      <c r="AJ4" s="90"/>
-      <c r="AK4" s="88">
+      <c r="AE4" s="86"/>
+      <c r="AF4" s="86"/>
+      <c r="AG4" s="86"/>
+      <c r="AH4" s="86"/>
+      <c r="AI4" s="86"/>
+      <c r="AJ4" s="87"/>
+      <c r="AK4" s="85">
         <f>AK5</f>
         <v>44150</v>
       </c>
-      <c r="AL4" s="89"/>
-      <c r="AM4" s="89"/>
-      <c r="AN4" s="89"/>
-      <c r="AO4" s="89"/>
-      <c r="AP4" s="89"/>
-      <c r="AQ4" s="90"/>
-      <c r="AR4" s="88">
+      <c r="AL4" s="86"/>
+      <c r="AM4" s="86"/>
+      <c r="AN4" s="86"/>
+      <c r="AO4" s="86"/>
+      <c r="AP4" s="86"/>
+      <c r="AQ4" s="87"/>
+      <c r="AR4" s="85">
         <f>AR5</f>
         <v>44157</v>
       </c>
-      <c r="AS4" s="89"/>
-      <c r="AT4" s="89"/>
-      <c r="AU4" s="89"/>
-      <c r="AV4" s="89"/>
-      <c r="AW4" s="89"/>
-      <c r="AX4" s="90"/>
-      <c r="AY4" s="88">
+      <c r="AS4" s="86"/>
+      <c r="AT4" s="86"/>
+      <c r="AU4" s="86"/>
+      <c r="AV4" s="86"/>
+      <c r="AW4" s="86"/>
+      <c r="AX4" s="87"/>
+      <c r="AY4" s="85">
         <f>AY5</f>
         <v>44164</v>
       </c>
-      <c r="AZ4" s="89"/>
-      <c r="BA4" s="89"/>
-      <c r="BB4" s="89"/>
-      <c r="BC4" s="89"/>
-      <c r="BD4" s="89"/>
-      <c r="BE4" s="90"/>
-      <c r="BF4" s="88">
+      <c r="AZ4" s="86"/>
+      <c r="BA4" s="86"/>
+      <c r="BB4" s="86"/>
+      <c r="BC4" s="86"/>
+      <c r="BD4" s="86"/>
+      <c r="BE4" s="87"/>
+      <c r="BF4" s="85">
         <f>BF5</f>
         <v>44171</v>
       </c>
-      <c r="BG4" s="89"/>
-      <c r="BH4" s="89"/>
-      <c r="BI4" s="89"/>
-      <c r="BJ4" s="89"/>
-      <c r="BK4" s="89"/>
-      <c r="BL4" s="90"/>
-    </row>
-    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="BG4" s="86"/>
+      <c r="BH4" s="86"/>
+      <c r="BI4" s="86"/>
+      <c r="BJ4" s="86"/>
+      <c r="BK4" s="86"/>
+      <c r="BL4" s="87"/>
+    </row>
+    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+1+7*(Display_Week-1)</f>
         <v>44122</v>
@@ -1910,7 +1910,7 @@
         <v>44177</v>
       </c>
     </row>
-    <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="39" t="s">
         <v>32</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="38" t="s">
         <v>27</v>
       </c>
@@ -2225,7 +2225,7 @@
       <c r="BK7" s="24"/>
       <c r="BL7" s="24"/>
     </row>
-    <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="39" t="s">
         <v>33</v>
       </c>
@@ -2309,7 +2309,7 @@
       <c r="BK8" s="24"/>
       <c r="BL8" s="24"/>
     </row>
-    <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="39" t="s">
         <v>34</v>
       </c>
@@ -2393,7 +2393,7 @@
       <c r="BK9" s="24"/>
       <c r="BL9" s="24"/>
     </row>
-    <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="39" t="s">
         <v>35</v>
       </c>
@@ -2477,7 +2477,7 @@
       <c r="BK10" s="24"/>
       <c r="BL10" s="24"/>
     </row>
-    <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="39"/>
       <c r="B11" s="54" t="s">
         <v>49</v>
@@ -2556,7 +2556,7 @@
       <c r="BK11" s="24"/>
       <c r="BL11" s="24"/>
     </row>
-    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="38"/>
       <c r="B12" s="54" t="s">
         <v>43</v>
@@ -2638,7 +2638,7 @@
       <c r="BK12" s="24"/>
       <c r="BL12" s="24"/>
     </row>
-    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="38"/>
       <c r="B13" s="54" t="s">
         <v>42</v>
@@ -2720,7 +2720,7 @@
       <c r="BK13" s="24"/>
       <c r="BL13" s="24"/>
     </row>
-    <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="38"/>
       <c r="B14" s="54" t="s">
         <v>44</v>
@@ -2799,7 +2799,7 @@
       <c r="BK14" s="24"/>
       <c r="BL14" s="24"/>
     </row>
-    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="38"/>
       <c r="B15" s="54" t="s">
         <v>45</v>
@@ -2881,7 +2881,7 @@
       <c r="BK15" s="24"/>
       <c r="BL15" s="24"/>
     </row>
-    <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="39" t="s">
         <v>36</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>7</v>
       </c>
       <c r="D16" s="60">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E16" s="61">
         <f>F15 + 1</f>
@@ -2965,7 +2965,7 @@
       <c r="BK16" s="24"/>
       <c r="BL16" s="24"/>
     </row>
-    <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="39"/>
       <c r="B17" s="63" t="s">
         <v>47</v>
@@ -3047,7 +3047,7 @@
       <c r="BK17" s="24"/>
       <c r="BL17" s="24"/>
     </row>
-    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="38"/>
       <c r="B18" s="63" t="s">
         <v>50</v>
@@ -3129,7 +3129,7 @@
       <c r="BK18" s="24"/>
       <c r="BL18" s="24"/>
     </row>
-    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="38"/>
       <c r="B19" s="63" t="s">
         <v>48</v>
@@ -3211,7 +3211,7 @@
       <c r="BK19" s="24"/>
       <c r="BL19" s="24"/>
     </row>
-    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="38"/>
       <c r="B20" s="63" t="s">
         <v>51</v>
@@ -3293,7 +3293,7 @@
       <c r="BK20" s="24"/>
       <c r="BL20" s="24"/>
     </row>
-    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="38"/>
       <c r="B21" s="63" t="s">
         <v>53</v>
@@ -3303,7 +3303,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="66">
         <f>E19+2</f>
@@ -3375,7 +3375,7 @@
       <c r="BK21" s="24"/>
       <c r="BL21" s="24"/>
     </row>
-    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="38" t="s">
         <v>24</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>6</v>
       </c>
       <c r="D22" s="69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="70">
         <f>F21+1</f>
@@ -3459,7 +3459,7 @@
       <c r="BK22" s="24"/>
       <c r="BL22" s="24"/>
     </row>
-    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="38"/>
       <c r="B23" s="72" t="s">
         <v>55</v>
@@ -3469,7 +3469,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="75">
         <f>E22</f>
@@ -3541,7 +3541,7 @@
       <c r="BK23" s="24"/>
       <c r="BL23" s="24"/>
     </row>
-    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="38"/>
       <c r="B24" s="72" t="s">
         <v>56</v>
@@ -3623,7 +3623,7 @@
       <c r="BK24" s="24"/>
       <c r="BL24" s="24"/>
     </row>
-    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="38"/>
       <c r="B25" s="72" t="s">
         <v>57</v>
@@ -3633,7 +3633,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="75">
         <f>E24+1</f>
@@ -3705,7 +3705,7 @@
       <c r="BK25" s="24"/>
       <c r="BL25" s="24"/>
     </row>
-    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="38"/>
       <c r="B26" s="72" t="s">
         <v>58</v>
@@ -3715,7 +3715,7 @@
         <v>4</v>
       </c>
       <c r="D26" s="74">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E26" s="75">
         <f>E24+1</f>
@@ -3787,7 +3787,7 @@
       <c r="BK26" s="24"/>
       <c r="BL26" s="24"/>
     </row>
-    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="38"/>
       <c r="B27" s="72" t="s">
         <v>59</v>
@@ -3797,7 +3797,7 @@
         <v>4</v>
       </c>
       <c r="D27" s="74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="75">
         <f>E25+1</f>
@@ -3866,7 +3866,7 @@
       <c r="BK27" s="24"/>
       <c r="BL27" s="24"/>
     </row>
-    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="38"/>
       <c r="B28" s="72" t="s">
         <v>60</v>
@@ -3876,7 +3876,7 @@
         <v>2</v>
       </c>
       <c r="D28" s="74">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E28" s="75">
         <f>E26+2</f>
@@ -3945,7 +3945,7 @@
       <c r="BK28" s="24"/>
       <c r="BL28" s="24"/>
     </row>
-    <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="38" t="s">
         <v>24</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>12</v>
       </c>
       <c r="D29" s="78">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="E29" s="79">
         <f>E28+2</f>
@@ -4029,7 +4029,7 @@
       <c r="BK29" s="24"/>
       <c r="BL29" s="24"/>
     </row>
-    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="38"/>
       <c r="B30" s="81" t="s">
         <v>61</v>
@@ -4039,7 +4039,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="84">
         <f>E29</f>
@@ -4111,7 +4111,7 @@
       <c r="BK30" s="24"/>
       <c r="BL30" s="24"/>
     </row>
-    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="38"/>
       <c r="B31" s="81" t="s">
         <v>63</v>
@@ -4193,7 +4193,7 @@
       <c r="BK31" s="24"/>
       <c r="BL31" s="24"/>
     </row>
-    <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="38"/>
       <c r="B32" s="81" t="s">
         <v>64</v>
@@ -4275,7 +4275,7 @@
       <c r="BK32" s="24"/>
       <c r="BL32" s="24"/>
     </row>
-    <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="38" t="s">
         <v>26</v>
       </c>
@@ -4346,7 +4346,7 @@
       <c r="BK33" s="24"/>
       <c r="BL33" s="24"/>
     </row>
-    <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="39" t="s">
         <v>25</v>
       </c>
@@ -4419,18 +4419,23 @@
       <c r="BK34" s="26"/>
       <c r="BL34" s="26"/>
     </row>
-    <row r="35" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C36" s="14"/>
       <c r="F36" s="40"/>
     </row>
-    <row r="37" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C37" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4438,11 +4443,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D26 D29:D34">
     <cfRule type="dataBar" priority="16">
@@ -4570,86 +4570,86 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.17578125" defaultRowHeight="13" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="87.17578125" style="28" customWidth="1"/>
-    <col min="2" max="16384" width="9.17578125" style="2"/>
+    <col min="1" max="1" width="87.1796875" style="28" customWidth="1"/>
+    <col min="2" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="1:2" s="30" customFormat="1" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:2" s="30" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="29"/>
     </row>
-    <row r="3" spans="1:2" s="34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" s="34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="35" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="35"/>
     </row>
-    <row r="4" spans="1:2" s="31" customFormat="1" ht="25.7" x14ac:dyDescent="0.85">
+    <row r="4" spans="1:2" s="31" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="A4" s="32" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="28" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:2" s="28" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="31" customFormat="1" ht="25.7" x14ac:dyDescent="0.85">
+    <row r="8" spans="1:2" s="31" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="A8" s="32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="43" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" ht="58" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="28" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:2" s="28" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="36" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="31" customFormat="1" ht="25.7" x14ac:dyDescent="0.85">
+    <row r="11" spans="1:2" s="31" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="A11" s="32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="28.7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="28" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:2" s="28" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="31" customFormat="1" ht="25.7" x14ac:dyDescent="0.85">
+    <row r="14" spans="1:2" s="31" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="A14" s="32" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="33" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="57.35" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" ht="72.5" x14ac:dyDescent="0.3">
       <c r="A16" s="33" t="s">
         <v>15</v>
       </c>

</xml_diff>